<commit_message>
Min refund calculation is altered
</commit_message>
<xml_diff>
--- a/testData/testDataGlobalBlue.xlsx
+++ b/testData/testDataGlobalBlue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="94">
   <si>
     <t>United Kingdom</t>
   </si>
@@ -280,6 +280,24 @@
   </si>
   <si>
     <t>Refund_amount</t>
+  </si>
+  <si>
+    <t>54001</t>
+  </si>
+  <si>
+    <t>6000</t>
+  </si>
+  <si>
+    <t>150000</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>10000</t>
   </si>
 </sst>
 </file>
@@ -503,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -517,6 +535,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -826,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -872,17 +893,17 @@
       <c r="I1" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="13"/>
+      <c r="K1" s="16"/>
       <c r="L1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="14"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
@@ -897,7 +918,7 @@
       <c r="D2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="13">
         <v>1000</v>
       </c>
       <c r="F2" s="9">
@@ -945,7 +966,7 @@
       <c r="D3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="14">
         <v>1000</v>
       </c>
       <c r="F3" s="2">
@@ -992,7 +1013,7 @@
       <c r="D4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="14">
         <v>1000</v>
       </c>
       <c r="F4" s="2">
@@ -1039,7 +1060,7 @@
       <c r="D5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="14">
         <v>1000</v>
       </c>
       <c r="F5" s="2">
@@ -1086,7 +1107,7 @@
       <c r="D6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="14">
         <v>1000</v>
       </c>
       <c r="F6" s="2">
@@ -1133,7 +1154,7 @@
       <c r="D7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="14">
         <v>1000</v>
       </c>
       <c r="F7" s="2">
@@ -1180,7 +1201,7 @@
       <c r="D8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="14">
         <v>1000</v>
       </c>
       <c r="F8" s="2">
@@ -1227,7 +1248,7 @@
       <c r="D9" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="14">
         <v>10000</v>
       </c>
       <c r="F9" s="2">
@@ -1274,7 +1295,7 @@
       <c r="D10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="14">
         <v>1000</v>
       </c>
       <c r="F10" s="2">
@@ -1321,7 +1342,7 @@
       <c r="D11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="14">
         <v>1000</v>
       </c>
       <c r="F11" s="2">
@@ -1368,7 +1389,7 @@
       <c r="D12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="14">
         <v>1000</v>
       </c>
       <c r="F12" s="2">
@@ -1415,7 +1436,7 @@
       <c r="D13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="14">
         <v>1000</v>
       </c>
       <c r="F13" s="2">
@@ -1462,7 +1483,7 @@
       <c r="D14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="14">
         <v>1000</v>
       </c>
       <c r="F14" s="2">
@@ -1509,7 +1530,7 @@
       <c r="D15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="14">
         <v>1000</v>
       </c>
       <c r="F15" s="2">
@@ -1556,19 +1577,19 @@
       <c r="D16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="2">
-        <v>20000</v>
-      </c>
-      <c r="F16" s="2">
-        <f t="shared" si="1"/>
-        <v>19999</v>
+      <c r="E16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="14">
+        <f>E16-1</f>
+        <v>54000</v>
       </c>
       <c r="G16" s="2">
         <v>27</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
-        <v>5400</v>
+        <v>14580.27</v>
       </c>
       <c r="I16" s="2">
         <v>-10</v>
@@ -1578,7 +1599,7 @@
       </c>
       <c r="K16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least Ft 20000</v>
+        <v>You need to purchase at least Ft 54001</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>81</v>
@@ -1603,19 +1624,19 @@
       <c r="D17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="2">
-        <v>1000</v>
+      <c r="E17" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="1"/>
-        <v>999</v>
+        <v>5999</v>
       </c>
       <c r="G17" s="2">
         <v>27</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>1620</v>
       </c>
       <c r="I17" s="2">
         <v>-10</v>
@@ -1625,7 +1646,7 @@
       </c>
       <c r="K17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least € 6000</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>81</v>
@@ -1650,7 +1671,7 @@
       <c r="D18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="14">
         <v>1000</v>
       </c>
       <c r="F18" s="2">
@@ -1697,7 +1718,7 @@
       <c r="D19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="14">
         <v>1000</v>
       </c>
       <c r="F19" s="2">
@@ -1744,7 +1765,7 @@
       <c r="D20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="14">
         <v>1000</v>
       </c>
       <c r="F20" s="2">
@@ -1791,7 +1812,7 @@
       <c r="D21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="14">
         <v>1000</v>
       </c>
       <c r="F21" s="2">
@@ -1838,19 +1859,19 @@
       <c r="D22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="2">
-        <v>1000</v>
+      <c r="E22" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="1"/>
-        <v>999</v>
+        <v>149999</v>
       </c>
       <c r="G22" s="2">
         <v>27</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>40500</v>
       </c>
       <c r="I22" s="2">
         <v>-10</v>
@@ -1860,7 +1881,7 @@
       </c>
       <c r="K22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least £ 1000</v>
+        <v>You need to purchase at least £ 150000</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>81</v>
@@ -1885,7 +1906,7 @@
       <c r="D23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="14">
         <v>1000</v>
       </c>
       <c r="F23" s="2">
@@ -1932,7 +1953,7 @@
       <c r="D24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="14">
         <v>1000</v>
       </c>
       <c r="F24" s="2">
@@ -1979,7 +2000,7 @@
       <c r="D25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="14">
         <v>1000</v>
       </c>
       <c r="F25" s="2">
@@ -2026,19 +2047,19 @@
       <c r="D26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="2">
-        <v>1000</v>
+      <c r="E26" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="1"/>
-        <v>999</v>
+        <v>1999</v>
       </c>
       <c r="G26" s="2">
         <v>27</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>540</v>
       </c>
       <c r="I26" s="2">
         <v>-10</v>
@@ -2048,7 +2069,7 @@
       </c>
       <c r="K26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least € 2000</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>81</v>
@@ -2073,7 +2094,7 @@
       <c r="D27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="14">
         <v>1000</v>
       </c>
       <c r="F27" s="2">
@@ -2120,7 +2141,7 @@
       <c r="D28" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="14">
         <v>1000</v>
       </c>
       <c r="F28" s="2">
@@ -2167,7 +2188,7 @@
       <c r="D29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="14">
         <v>1000</v>
       </c>
       <c r="F29" s="2">
@@ -2214,7 +2235,7 @@
       <c r="D30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="14">
         <v>1000</v>
       </c>
       <c r="F30" s="2">
@@ -2261,19 +2282,19 @@
       <c r="D31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="2">
-        <v>1000</v>
+      <c r="E31" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="1"/>
-        <v>999</v>
+        <v>29999</v>
       </c>
       <c r="G31" s="2">
         <v>27</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>8100.0000000000009</v>
       </c>
       <c r="I31" s="2">
         <v>-10</v>
@@ -2283,7 +2304,7 @@
       </c>
       <c r="K31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least € 30000</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>81</v>
@@ -2308,19 +2329,19 @@
       <c r="D32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="2">
-        <v>1000</v>
+      <c r="E32" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="1"/>
-        <v>999</v>
+        <v>9999</v>
       </c>
       <c r="G32" s="2">
         <v>27</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>2700</v>
       </c>
       <c r="I32" s="2">
         <v>-10</v>
@@ -2330,7 +2351,7 @@
       </c>
       <c r="K32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least € 10000</v>
       </c>
       <c r="L32" s="2" t="s">
         <v>81</v>
@@ -2355,7 +2376,7 @@
       <c r="D33" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="14">
         <v>1000</v>
       </c>
       <c r="F33" s="2">
@@ -2402,7 +2423,7 @@
       <c r="D34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="14">
         <v>1000</v>
       </c>
       <c r="F34" s="2">
@@ -2449,7 +2470,7 @@
       <c r="D35" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="14">
         <v>1000</v>
       </c>
       <c r="F35" s="2">
@@ -2496,7 +2517,7 @@
       <c r="D36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="14">
         <v>1000</v>
       </c>
       <c r="F36" s="2">
@@ -2543,7 +2564,7 @@
       <c r="D37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="14">
         <v>1000</v>
       </c>
       <c r="F37" s="2">
@@ -2590,7 +2611,7 @@
       <c r="D38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="14">
         <v>1000</v>
       </c>
       <c r="F38" s="2">
@@ -2637,7 +2658,7 @@
       <c r="D39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="14">
         <v>1000</v>
       </c>
       <c r="F39" s="2">
@@ -2684,7 +2705,7 @@
       <c r="D40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="14">
         <v>1000</v>
       </c>
       <c r="F40" s="2">
@@ -2731,7 +2752,7 @@
       <c r="D41" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="15">
         <v>1000</v>
       </c>
       <c r="F41" s="6">

</xml_diff>

<commit_message>
Cucumber scenario implementation added
</commit_message>
<xml_diff>
--- a/testData/testDataGlobalBlue.xlsx
+++ b/testData/testDataGlobalBlue.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="101">
   <si>
     <t>United Kingdom</t>
   </si>
@@ -231,33 +231,6 @@
     <t>Currency_symbol</t>
   </si>
   <si>
-    <t>€</t>
-  </si>
-  <si>
-    <t>$</t>
-  </si>
-  <si>
-    <t>kr</t>
-  </si>
-  <si>
-    <t>Ft</t>
-  </si>
-  <si>
-    <t>Fr.</t>
-  </si>
-  <si>
-    <t>₺</t>
-  </si>
-  <si>
-    <t>¥</t>
-  </si>
-  <si>
-    <t>£</t>
-  </si>
-  <si>
-    <t>$U</t>
-  </si>
-  <si>
     <t>Not_Numeric_Value</t>
   </si>
   <si>
@@ -298,6 +271,54 @@
   </si>
   <si>
     <t>10000</t>
+  </si>
+  <si>
+    <t>($)</t>
+  </si>
+  <si>
+    <t>(€)</t>
+  </si>
+  <si>
+    <t>(¥)</t>
+  </si>
+  <si>
+    <t>(kn)</t>
+  </si>
+  <si>
+    <t>(Kč)</t>
+  </si>
+  <si>
+    <t>(kr)</t>
+  </si>
+  <si>
+    <t>(Ft)</t>
+  </si>
+  <si>
+    <t>(£)</t>
+  </si>
+  <si>
+    <t>(RM)</t>
+  </si>
+  <si>
+    <t>(MAD)</t>
+  </si>
+  <si>
+    <t>(zł)</t>
+  </si>
+  <si>
+    <t>(₩)</t>
+  </si>
+  <si>
+    <t>(₽)</t>
+  </si>
+  <si>
+    <t>(Fr.)</t>
+  </si>
+  <si>
+    <t>(₺)</t>
+  </si>
+  <si>
+    <t>($U)</t>
   </si>
 </sst>
 </file>
@@ -847,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,23 +906,23 @@
         <v>67</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>69</v>
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="12" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="N1" s="17"/>
     </row>
@@ -916,7 +937,7 @@
         <v>43</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E2" s="13">
         <v>1000</v>
@@ -926,11 +947,11 @@
         <v>999</v>
       </c>
       <c r="G2" s="9">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H2" s="9">
         <f>E2*(G2/100)</f>
-        <v>270</v>
+        <v>130</v>
       </c>
       <c r="I2" s="9">
         <v>-10</v>
@@ -940,16 +961,16 @@
       </c>
       <c r="K2" s="9" t="str">
         <f t="shared" ref="K2:K41" si="0">CONCATENATE("You need to purchase at least ", D2," ", E2)</f>
-        <v>You need to purchase at least $ 1000</v>
+        <v>You need to purchase at least ($) 1000</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="1"/>
     </row>
@@ -964,7 +985,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E3" s="14">
         <v>1000</v>
@@ -974,11 +995,11 @@
         <v>999</v>
       </c>
       <c r="G3" s="2">
-        <v>28</v>
+        <v>12.5</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ref="H3:H41" si="2">E3*(G3/100)</f>
-        <v>280</v>
+        <v>125</v>
       </c>
       <c r="I3" s="2">
         <v>-10</v>
@@ -988,16 +1009,16 @@
       </c>
       <c r="K3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1011,7 +1032,7 @@
         <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E4" s="14">
         <v>1000</v>
@@ -1021,11 +1042,11 @@
         <v>999</v>
       </c>
       <c r="G4" s="2">
-        <v>18</v>
+        <v>5.93</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>59.3</v>
       </c>
       <c r="I4" s="2">
         <v>-10</v>
@@ -1035,16 +1056,16 @@
       </c>
       <c r="K4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least ($) 1000</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1058,7 +1079,7 @@
         <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E5" s="14">
         <v>1000</v>
@@ -1068,11 +1089,11 @@
         <v>999</v>
       </c>
       <c r="G5" s="2">
-        <v>30</v>
+        <v>11.8</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>118.00000000000001</v>
       </c>
       <c r="I5" s="2">
         <v>-10</v>
@@ -1082,16 +1103,16 @@
       </c>
       <c r="K5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -1105,7 +1126,7 @@
         <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="E6" s="14">
         <v>1000</v>
@@ -1115,11 +1136,11 @@
         <v>999</v>
       </c>
       <c r="G6" s="2">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="I6" s="2">
         <v>-10</v>
@@ -1129,16 +1150,16 @@
       </c>
       <c r="K6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (¥) 1000</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
@@ -1152,7 +1173,7 @@
         <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="E7" s="14">
         <v>1000</v>
@@ -1162,11 +1183,11 @@
         <v>999</v>
       </c>
       <c r="G7" s="2">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>150</v>
       </c>
       <c r="I7" s="2">
         <v>-10</v>
@@ -1176,16 +1197,16 @@
       </c>
       <c r="K7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (kn) 1000</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1199,7 +1220,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E8" s="14">
         <v>1000</v>
@@ -1209,11 +1230,11 @@
         <v>999</v>
       </c>
       <c r="G8" s="2">
-        <v>28</v>
+        <v>11.3</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>113</v>
       </c>
       <c r="I8" s="2">
         <v>-10</v>
@@ -1223,16 +1244,16 @@
       </c>
       <c r="K8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1246,7 +1267,7 @@
         <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="E9" s="14">
         <v>10000</v>
@@ -1256,11 +1277,11 @@
         <v>9999</v>
       </c>
       <c r="G9" s="2">
-        <v>18</v>
+        <v>11.7</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="2"/>
-        <v>1800</v>
+        <v>1170</v>
       </c>
       <c r="I9" s="2">
         <v>-10</v>
@@ -1270,16 +1291,16 @@
       </c>
       <c r="K9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 10000</v>
+        <v>You need to purchase at least (Kč) 10000</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1293,7 +1314,7 @@
         <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="E10" s="14">
         <v>1000</v>
@@ -1303,11 +1324,11 @@
         <v>999</v>
       </c>
       <c r="G10" s="2">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>130</v>
       </c>
       <c r="I10" s="2">
         <v>-10</v>
@@ -1317,16 +1338,16 @@
       </c>
       <c r="K10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least kr 1000</v>
+        <v>You need to purchase at least (kr) 1000</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1340,7 +1361,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E11" s="14">
         <v>1000</v>
@@ -1350,11 +1371,11 @@
         <v>999</v>
       </c>
       <c r="G11" s="2">
-        <v>27</v>
+        <v>11.5</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="2"/>
-        <v>270</v>
+        <f>E11*(G11/100)</f>
+        <v>115</v>
       </c>
       <c r="I11" s="2">
         <v>-10</v>
@@ -1364,16 +1385,16 @@
       </c>
       <c r="K11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1387,7 +1408,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E12" s="14">
         <v>1000</v>
@@ -1397,11 +1418,11 @@
         <v>999</v>
       </c>
       <c r="G12" s="2">
-        <v>27</v>
+        <v>13.5</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>135</v>
       </c>
       <c r="I12" s="2">
         <v>-10</v>
@@ -1411,16 +1432,16 @@
       </c>
       <c r="K12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1434,7 +1455,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E13" s="14">
         <v>1000</v>
@@ -1444,11 +1465,11 @@
         <v>999</v>
       </c>
       <c r="G13" s="2">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>120</v>
       </c>
       <c r="I13" s="2">
         <v>-10</v>
@@ -1458,16 +1479,16 @@
       </c>
       <c r="K13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -1481,7 +1502,7 @@
         <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E14" s="14">
         <v>1000</v>
@@ -1491,11 +1512,11 @@
         <v>999</v>
       </c>
       <c r="G14" s="2">
-        <v>18</v>
+        <v>11.4</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="I14" s="2">
         <v>-10</v>
@@ -1505,16 +1526,16 @@
       </c>
       <c r="K14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -1528,7 +1549,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E15" s="14">
         <v>1000</v>
@@ -1538,11 +1559,11 @@
         <v>999</v>
       </c>
       <c r="G15" s="2">
-        <v>30</v>
+        <v>12.4</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>124</v>
       </c>
       <c r="I15" s="2">
         <v>-10</v>
@@ -1552,16 +1573,16 @@
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -1575,21 +1596,21 @@
         <v>50</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="F16" s="14">
         <f>E16-1</f>
         <v>54000</v>
       </c>
       <c r="G16" s="2">
-        <v>27</v>
+        <v>14.258995000000001</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
-        <v>14580.27</v>
+        <v>7699.9998899499997</v>
       </c>
       <c r="I16" s="2">
         <v>-10</v>
@@ -1599,16 +1620,16 @@
       </c>
       <c r="K16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least Ft 54001</v>
+        <v>You need to purchase at least (Ft) 54001</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1622,21 +1643,21 @@
         <v>51</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="1"/>
         <v>5999</v>
       </c>
       <c r="G17" s="2">
-        <v>27</v>
+        <v>14.166667</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="2"/>
-        <v>1620</v>
+        <v>850.00001999999995</v>
       </c>
       <c r="I17" s="2">
         <v>-10</v>
@@ -1646,16 +1667,16 @@
       </c>
       <c r="K17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 6000</v>
+        <v>You need to purchase at least (kr) 6000</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1669,7 +1690,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E18" s="14">
         <v>1000</v>
@@ -1679,11 +1700,11 @@
         <v>999</v>
       </c>
       <c r="G18" s="2">
-        <v>28</v>
+        <v>13.9</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>139</v>
       </c>
       <c r="I18" s="2">
         <v>-10</v>
@@ -1693,16 +1714,16 @@
       </c>
       <c r="K18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1716,7 +1737,7 @@
         <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E19" s="14">
         <v>1000</v>
@@ -1726,11 +1747,11 @@
         <v>999</v>
       </c>
       <c r="G19" s="2">
-        <v>18</v>
+        <v>12.9</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="I19" s="2">
         <v>-10</v>
@@ -1740,16 +1761,16 @@
       </c>
       <c r="K19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
@@ -1763,7 +1784,7 @@
         <v>52</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="E20" s="14">
         <v>1000</v>
@@ -1773,11 +1794,11 @@
         <v>999</v>
       </c>
       <c r="G20" s="2">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="I20" s="2">
         <v>-10</v>
@@ -1787,16 +1808,16 @@
       </c>
       <c r="K20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least ¥ 1000</v>
+        <v>You need to purchase at least (¥) 1000</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
@@ -1810,7 +1831,7 @@
         <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E21" s="14">
         <v>1000</v>
@@ -1820,11 +1841,11 @@
         <v>999</v>
       </c>
       <c r="G21" s="2">
-        <v>27</v>
+        <v>12.397</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>123.97</v>
       </c>
       <c r="I21" s="2">
         <v>-10</v>
@@ -1834,16 +1855,16 @@
       </c>
       <c r="K21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -1857,21 +1878,21 @@
         <v>53</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="1"/>
         <v>149999</v>
       </c>
       <c r="G22" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>40500</v>
+        <v>12000</v>
       </c>
       <c r="I22" s="2">
         <v>-10</v>
@@ -1881,16 +1902,16 @@
       </c>
       <c r="K22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least £ 150000</v>
+        <v>You need to purchase at least (£) 150000</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1904,7 +1925,7 @@
         <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E23" s="14">
         <v>1000</v>
@@ -1914,11 +1935,11 @@
         <v>999</v>
       </c>
       <c r="G23" s="2">
-        <v>28</v>
+        <v>12.2</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>122</v>
       </c>
       <c r="I23" s="2">
         <v>-10</v>
@@ -1928,16 +1949,16 @@
       </c>
       <c r="K23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
@@ -1951,7 +1972,7 @@
         <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E24" s="14">
         <v>1000</v>
@@ -1961,11 +1982,11 @@
         <v>999</v>
       </c>
       <c r="G24" s="2">
-        <v>18</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>98</v>
       </c>
       <c r="I24" s="2">
         <v>-10</v>
@@ -1975,16 +1996,16 @@
       </c>
       <c r="K24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
@@ -1998,7 +2019,7 @@
         <v>54</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="E25" s="14">
         <v>1000</v>
@@ -2008,11 +2029,11 @@
         <v>999</v>
       </c>
       <c r="G25" s="2">
-        <v>30</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>48.099999999999994</v>
       </c>
       <c r="I25" s="2">
         <v>-10</v>
@@ -2022,16 +2043,16 @@
       </c>
       <c r="K25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (RM) 1000</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
@@ -2045,21 +2066,21 @@
         <v>55</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="1"/>
         <v>1999</v>
       </c>
       <c r="G26" s="2">
-        <v>27</v>
+        <v>12.75</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="2"/>
-        <v>540</v>
+        <v>255</v>
       </c>
       <c r="I26" s="2">
         <v>-10</v>
@@ -2069,16 +2090,16 @@
       </c>
       <c r="K26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 2000</v>
+        <v>You need to purchase at least (MAD) 2000</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -2092,7 +2113,7 @@
         <v>44</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E27" s="14">
         <v>1000</v>
@@ -2102,11 +2123,11 @@
         <v>999</v>
       </c>
       <c r="G27" s="2">
-        <v>27</v>
+        <v>11.2</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>111.99999999999999</v>
       </c>
       <c r="I27" s="2">
         <v>-10</v>
@@ -2116,16 +2137,16 @@
       </c>
       <c r="K27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -2139,7 +2160,7 @@
         <v>64</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E28" s="14">
         <v>1000</v>
@@ -2149,11 +2170,11 @@
         <v>999</v>
       </c>
       <c r="G28" s="2">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>120</v>
       </c>
       <c r="I28" s="2">
         <v>-10</v>
@@ -2163,16 +2184,16 @@
       </c>
       <c r="K28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (kr) 1000</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
@@ -2186,7 +2207,7 @@
         <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="E29" s="14">
         <v>1000</v>
@@ -2196,11 +2217,11 @@
         <v>999</v>
       </c>
       <c r="G29" s="2">
-        <v>18</v>
+        <v>13.6</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="I29" s="2">
         <v>-10</v>
@@ -2210,16 +2231,16 @@
       </c>
       <c r="K29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (zł) 1000</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
@@ -2233,7 +2254,7 @@
         <v>44</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E30" s="14">
         <v>1000</v>
@@ -2243,11 +2264,11 @@
         <v>999</v>
       </c>
       <c r="G30" s="2">
-        <v>30</v>
+        <v>13.9</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>139</v>
       </c>
       <c r="I30" s="2">
         <v>-10</v>
@@ -2257,16 +2278,16 @@
       </c>
       <c r="K30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
@@ -2280,21 +2301,21 @@
         <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="1"/>
         <v>29999</v>
       </c>
       <c r="G31" s="2">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="2"/>
-        <v>8100.0000000000009</v>
+        <v>1500</v>
       </c>
       <c r="I31" s="2">
         <v>-10</v>
@@ -2304,16 +2325,16 @@
       </c>
       <c r="K31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 30000</v>
+        <v>You need to purchase at least (₩) 30000</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
@@ -2327,21 +2348,21 @@
         <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="1"/>
         <v>9999</v>
       </c>
       <c r="G32" s="2">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="2"/>
-        <v>2700</v>
+        <v>1100</v>
       </c>
       <c r="I32" s="2">
         <v>-10</v>
@@ -2351,16 +2372,16 @@
       </c>
       <c r="K32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 10000</v>
+        <v>You need to purchase at least (₽) 10000</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
@@ -2374,7 +2395,7 @@
         <v>59</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="E33" s="14">
         <v>1000</v>
@@ -2384,11 +2405,11 @@
         <v>999</v>
       </c>
       <c r="G33" s="2">
-        <v>28</v>
+        <v>5.5</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>55</v>
       </c>
       <c r="I33" s="2">
         <v>-10</v>
@@ -2398,16 +2419,16 @@
       </c>
       <c r="K33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least ($) 1000</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
@@ -2421,7 +2442,7 @@
         <v>44</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E34" s="14">
         <v>1000</v>
@@ -2431,11 +2452,11 @@
         <v>999</v>
       </c>
       <c r="G34" s="2">
-        <v>18</v>
+        <v>11.4</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="I34" s="2">
         <v>-10</v>
@@ -2445,16 +2466,16 @@
       </c>
       <c r="K34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
@@ -2468,7 +2489,7 @@
         <v>44</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E35" s="14">
         <v>1000</v>
@@ -2478,11 +2499,11 @@
         <v>999</v>
       </c>
       <c r="G35" s="2">
-        <v>30</v>
+        <v>14.5</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>145</v>
       </c>
       <c r="I35" s="2">
         <v>-10</v>
@@ -2492,16 +2513,16 @@
       </c>
       <c r="K35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -2515,7 +2536,7 @@
         <v>44</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="E36" s="14">
         <v>1000</v>
@@ -2525,11 +2546,11 @@
         <v>999</v>
       </c>
       <c r="G36" s="2">
-        <v>27</v>
+        <v>12.85</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>128.5</v>
       </c>
       <c r="I36" s="2">
         <v>-10</v>
@@ -2539,16 +2560,16 @@
       </c>
       <c r="K36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (€) 1000</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
@@ -2562,7 +2583,7 @@
         <v>60</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E37" s="14">
         <v>1000</v>
@@ -2572,11 +2593,11 @@
         <v>999</v>
       </c>
       <c r="G37" s="2">
-        <v>27</v>
+        <v>11.8</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>118.00000000000001</v>
       </c>
       <c r="I37" s="2">
         <v>-10</v>
@@ -2586,16 +2607,16 @@
       </c>
       <c r="K37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least € 1000</v>
+        <v>You need to purchase at least (kr) 1000</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
@@ -2609,7 +2630,7 @@
         <v>61</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="E38" s="14">
         <v>1000</v>
@@ -2619,11 +2640,11 @@
         <v>999</v>
       </c>
       <c r="G38" s="2">
-        <v>28</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="2"/>
-        <v>280</v>
+        <v>46</v>
       </c>
       <c r="I38" s="2">
         <v>-10</v>
@@ -2633,16 +2654,16 @@
       </c>
       <c r="K38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least Fr. 1000</v>
+        <v>You need to purchase at least (Fr.) 1000</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
@@ -2656,7 +2677,7 @@
         <v>62</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E39" s="14">
         <v>1000</v>
@@ -2666,11 +2687,11 @@
         <v>999</v>
       </c>
       <c r="G39" s="2">
-        <v>18</v>
+        <v>4.0750000000000002</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>40.75</v>
       </c>
       <c r="I39" s="2">
         <v>-10</v>
@@ -2680,16 +2701,16 @@
       </c>
       <c r="K39" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least ₺ 1000</v>
+        <v>You need to purchase at least (₺) 1000</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
@@ -2703,7 +2724,7 @@
         <v>65</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="E40" s="14">
         <v>1000</v>
@@ -2713,11 +2734,11 @@
         <v>999</v>
       </c>
       <c r="G40" s="2">
-        <v>30</v>
+        <v>12.2</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" si="2"/>
-        <v>300</v>
+        <v>122</v>
       </c>
       <c r="I40" s="2">
         <v>-10</v>
@@ -2727,16 +2748,16 @@
       </c>
       <c r="K40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least £ 1000</v>
+        <v>You need to purchase at least (£) 1000</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2750,7 +2771,7 @@
         <v>63</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E41" s="15">
         <v>1000</v>
@@ -2760,11 +2781,11 @@
         <v>999</v>
       </c>
       <c r="G41" s="6">
-        <v>27</v>
+        <v>14.426</v>
       </c>
       <c r="H41" s="6">
         <f t="shared" si="2"/>
-        <v>270</v>
+        <v>144.26</v>
       </c>
       <c r="I41" s="6">
         <v>-10</v>
@@ -2774,16 +2795,16 @@
       </c>
       <c r="K41" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>You need to purchase at least $U 1000</v>
+        <v>You need to purchase at least ($U) 1000</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M41" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N41" s="7" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>